<commit_message>
Working version with docstring and params for filenames
</commit_message>
<xml_diff>
--- a/std.xlsx
+++ b/std.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="460" windowWidth="26700" windowHeight="15320"/>
+    <workbookView xWindow="15000" yWindow="460" windowWidth="18420" windowHeight="8860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,10 +94,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -106,9 +115,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F15:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="I15" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -532,63 +542,63 @@
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1">
-        <v>21.542999999999999</v>
+        <v>41.542999999999999</v>
       </c>
       <c r="M18">
         <f>(J18-I18)/L18*100*10^3</f>
-        <v>972.47365733649008</v>
+        <v>504.2967527621982</v>
       </c>
       <c r="N18">
         <f>1001*10^3*G18/L18</f>
-        <v>878.19245230469301</v>
+        <v>455.40524276051326</v>
       </c>
       <c r="O18">
         <f>100*10^3*(I18-H18)/L18</f>
-        <v>957.61964443206625</v>
+        <v>496.59389066750123</v>
       </c>
       <c r="P18">
         <f>10*10^3*(H18-G18)/L18</f>
-        <v>196.72283340296153</v>
+        <v>102.0147798666442</v>
       </c>
       <c r="Q18">
         <f>50*10^3*(H18-G18)/L18</f>
-        <v>983.61416701480744</v>
+        <v>510.07389933322094</v>
       </c>
       <c r="R18">
         <f>100*10^3*(H18-G18)/L18</f>
-        <v>1967.2283340296149</v>
+        <v>1020.1477986664419</v>
       </c>
     </row>
     <row r="19" spans="7:18" x14ac:dyDescent="0.2">
       <c r="K19" s="1">
         <v>20.992999999999999</v>
       </c>
-      <c r="L19" s="1">
+      <c r="L19" s="2">
         <v>42.158499999999997</v>
       </c>
       <c r="M19">
         <f>K19/L19*M18</f>
-        <v>484.24729268035946</v>
+        <v>251.11666047740852</v>
       </c>
       <c r="N19">
         <f>N18*K19/L19</f>
-        <v>437.29957544107168</v>
+        <v>226.7709302103124</v>
       </c>
       <c r="O19">
         <f>K19/L19*O18</f>
-        <v>476.85067532199594</v>
+        <v>247.28098833646484</v>
       </c>
       <c r="P19">
         <f>P18*K19/L19</f>
-        <v>97.958951139826397</v>
+        <v>50.798682916623264</v>
       </c>
       <c r="Q19">
         <f>K19/L19*Q18</f>
-        <v>489.79475569913188</v>
+        <v>253.99341458311625</v>
       </c>
       <c r="R19">
         <f>R18*K19/L19</f>
-        <v>979.58951139826388</v>
+        <v>507.98682916623255</v>
       </c>
     </row>
     <row r="20" spans="7:18" x14ac:dyDescent="0.2">
@@ -601,27 +611,27 @@
       </c>
       <c r="M20">
         <f t="shared" ref="M20:M27" si="1">K20/L20*M19</f>
-        <v>225.14840645169193</v>
+        <v>116.75546109305535</v>
       </c>
       <c r="N20">
         <f t="shared" ref="N20:N27" si="2">N19*K20/L20</f>
-        <v>203.32029531355198</v>
+        <v>105.43603307271624</v>
       </c>
       <c r="O20">
         <f t="shared" ref="O20:O27" si="3">K20/L20*O19</f>
-        <v>221.70938544622453</v>
+        <v>114.97208412170559</v>
       </c>
       <c r="P20">
         <f t="shared" ref="P20:P27" si="4">P19*K20/L20</f>
-        <v>45.54553444115848</v>
+        <v>23.618598764313536</v>
       </c>
       <c r="Q20">
         <f t="shared" ref="Q20:Q27" si="5">K20/L20*Q19</f>
-        <v>227.72767220579235</v>
+        <v>118.09299382156765</v>
       </c>
       <c r="R20">
         <f t="shared" ref="R20:R27" si="6">R19*K20/L20</f>
-        <v>455.4553444115848</v>
+        <v>236.18598764313529</v>
       </c>
     </row>
     <row r="21" spans="7:18" x14ac:dyDescent="0.2">
@@ -634,27 +644,27 @@
       </c>
       <c r="M21">
         <f t="shared" si="1"/>
-        <v>111.35566666961283</v>
+        <v>57.745832680920223</v>
       </c>
       <c r="N21">
         <f t="shared" si="2"/>
-        <v>100.55974807425957</v>
+        <v>52.147381093415838</v>
       </c>
       <c r="O21">
         <f t="shared" si="3"/>
-        <v>109.6547686584302</v>
+        <v>56.863796095817868</v>
       </c>
       <c r="P21">
         <f t="shared" si="4"/>
-        <v>22.526268035599958</v>
+        <v>11.6814720239494</v>
       </c>
       <c r="Q21">
         <f t="shared" si="5"/>
-        <v>112.63134017799976</v>
+        <v>58.407360119746983</v>
       </c>
       <c r="R21">
         <f t="shared" si="6"/>
-        <v>225.26268035599955</v>
+        <v>116.81472023949397</v>
       </c>
     </row>
     <row r="22" spans="7:18" x14ac:dyDescent="0.2">
@@ -667,27 +677,27 @@
       </c>
       <c r="M22">
         <f t="shared" si="1"/>
-        <v>57.710105706990397</v>
+        <v>29.926794098781841</v>
       </c>
       <c r="N22">
         <f t="shared" si="2"/>
-        <v>52.115117845345139</v>
+        <v>27.02539498212143</v>
       </c>
       <c r="O22">
         <f t="shared" si="3"/>
-        <v>56.82861483222969</v>
+        <v>29.46967838939711</v>
       </c>
       <c r="P22">
         <f t="shared" si="4"/>
-        <v>11.674244772612186</v>
+        <v>6.0539261761640786</v>
       </c>
       <c r="Q22">
         <f t="shared" si="5"/>
-        <v>58.371223863060912</v>
+        <v>30.269630880820383</v>
       </c>
       <c r="R22">
         <f t="shared" si="6"/>
-        <v>116.74244772612184</v>
+        <v>60.539261761640773</v>
       </c>
     </row>
     <row r="23" spans="7:18" x14ac:dyDescent="0.2">
@@ -700,27 +710,27 @@
       </c>
       <c r="M23">
         <f t="shared" si="1"/>
-        <v>28.284849463987833</v>
+        <v>14.667706039590058</v>
       </c>
       <c r="N23">
         <f t="shared" si="2"/>
-        <v>25.542636683734578</v>
+        <v>13.245673689374723</v>
       </c>
       <c r="O23">
         <f t="shared" si="3"/>
-        <v>27.852813577187064</v>
+        <v>14.443664706288446</v>
       </c>
       <c r="P23">
         <f t="shared" si="4"/>
-        <v>5.7217752758176816</v>
+        <v>2.967147407913254</v>
       </c>
       <c r="Q23">
         <f t="shared" si="5"/>
-        <v>28.608876379088397</v>
+        <v>14.835737039566265</v>
       </c>
       <c r="R23">
         <f t="shared" si="6"/>
-        <v>57.217752758176808</v>
+        <v>29.671474079132533</v>
       </c>
     </row>
     <row r="24" spans="7:18" x14ac:dyDescent="0.2">
@@ -732,27 +742,27 @@
       </c>
       <c r="M24">
         <f t="shared" si="1"/>
-        <v>13.83455481603384</v>
+        <v>7.1742005729441063</v>
       </c>
       <c r="N24">
         <f t="shared" si="2"/>
-        <v>12.49329637752089</v>
+        <v>6.4786626835070305</v>
       </c>
       <c r="O24">
         <f t="shared" si="3"/>
-        <v>13.623239420275807</v>
+        <v>7.0646185116867271</v>
       </c>
       <c r="P24">
         <f t="shared" si="4"/>
-        <v>2.7986082725704731</v>
+        <v>1.4512774237774284</v>
       </c>
       <c r="Q24">
         <f t="shared" si="5"/>
-        <v>13.993041362852361</v>
+        <v>7.2563871188871394</v>
       </c>
       <c r="R24">
         <f t="shared" si="6"/>
-        <v>27.986082725704726</v>
+        <v>14.512774237774281</v>
       </c>
     </row>
     <row r="25" spans="7:18" x14ac:dyDescent="0.2">
@@ -764,27 +774,27 @@
       </c>
       <c r="M25">
         <f t="shared" si="1"/>
-        <v>7.0229684717657177</v>
+        <v>3.6419086196771739</v>
       </c>
       <c r="N25">
         <f t="shared" si="2"/>
-        <v>6.3420925164910962</v>
+        <v>3.288826013594774</v>
       </c>
       <c r="O25">
         <f t="shared" si="3"/>
-        <v>6.9156963996432825</v>
+        <v>3.5862804211904589</v>
       </c>
       <c r="P25">
         <f t="shared" si="4"/>
-        <v>1.4206845051715089</v>
+        <v>0.73672595370844229</v>
       </c>
       <c r="Q25">
         <f t="shared" si="5"/>
-        <v>7.1034225258575416</v>
+        <v>3.6836297685422097</v>
       </c>
       <c r="R25">
         <f t="shared" si="6"/>
-        <v>14.206845051715087</v>
+        <v>7.3672595370844212</v>
       </c>
     </row>
     <row r="26" spans="7:18" x14ac:dyDescent="0.2">
@@ -797,27 +807,27 @@
       </c>
       <c r="M26">
         <f t="shared" si="1"/>
-        <v>3.4809912277548598</v>
+        <v>1.8051415164894913</v>
       </c>
       <c r="N26">
         <f t="shared" si="2"/>
-        <v>3.1435095436167741</v>
+        <v>1.6301332618765179</v>
       </c>
       <c r="O26">
         <f t="shared" si="3"/>
-        <v>3.4278209560182704</v>
+        <v>1.7775689491731843</v>
       </c>
       <c r="P26">
         <f t="shared" si="4"/>
-        <v>0.70417378631146044</v>
+        <v>0.36516418839534437</v>
       </c>
       <c r="Q26">
         <f t="shared" si="5"/>
-        <v>3.5208689315573007</v>
+        <v>1.8258209419767211</v>
       </c>
       <c r="R26">
         <f t="shared" si="6"/>
-        <v>7.0417378631146024</v>
+        <v>3.651641883953443</v>
       </c>
     </row>
     <row r="27" spans="7:18" x14ac:dyDescent="0.2">
@@ -830,27 +840,27 @@
       </c>
       <c r="M27">
         <f t="shared" si="1"/>
-        <v>1.7199483192602067</v>
+        <v>0.89191552468099633</v>
       </c>
       <c r="N27">
         <f t="shared" si="2"/>
-        <v>1.5531995349523593</v>
+        <v>0.80544442099700742</v>
       </c>
       <c r="O27">
         <f t="shared" si="3"/>
-        <v>1.69367703228344</v>
+        <v>0.87829199399374491</v>
       </c>
       <c r="P27">
         <f t="shared" si="4"/>
-        <v>0.34793035689855639</v>
+        <v>0.18042663453928701</v>
       </c>
       <c r="Q27">
         <f t="shared" si="5"/>
-        <v>1.7396517844927812</v>
+        <v>0.90213317269643456</v>
       </c>
       <c r="R27">
         <f t="shared" si="6"/>
-        <v>3.4793035689855625</v>
+        <v>1.8042663453928698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>